<commit_message>
Add EM and topic list
</commit_message>
<xml_diff>
--- a/STA 663L-2.xlsx
+++ b/STA 663L-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26900" windowHeight="19080"/>
+    <workbookView xWindow="14540" yWindow="0" windowWidth="26900" windowHeight="19080"/>
   </bookViews>
   <sheets>
     <sheet name="ps" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="31">
   <si>
     <t>Permission</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Dropped</t>
+  </si>
+  <si>
+    <t>Zhe GAN</t>
+  </si>
+  <si>
+    <t>Sayan Patra</t>
   </si>
 </sst>
 </file>
@@ -956,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1517,7 +1523,9 @@
         <v>15</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="4">
         <v>42025</v>
@@ -1544,7 +1552,9 @@
         <v>15</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="4">
         <v>42025</v>

</xml_diff>

<commit_message>
Partial Exercise03 for lab
</commit_message>
<xml_diff>
--- a/STA 663L-2.xlsx
+++ b/STA 663L-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22820" yWindow="2680" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="12920" yWindow="1240" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="ps" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="35">
   <si>
     <t>Permission</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>chunyuan.li@duke.edu</t>
   </si>
 </sst>
 </file>
@@ -606,7 +609,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -653,6 +656,10 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -669,7 +676,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -700,6 +707,8 @@
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -707,6 +716,8 @@
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -985,7 +996,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -996,7 +1007,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1409,7 +1420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" ht="28">
       <c r="A14" s="3">
         <v>659665</v>
       </c>
@@ -1421,7 +1432,9 @@
         <v>15</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="4">
         <v>42025</v>
@@ -1448,7 +1461,9 @@
         <v>15</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="4">
         <v>42025</v>

</xml_diff>